<commit_message>
Cleaned out the use of configobj
</commit_message>
<xml_diff>
--- a/TPV_Source/test2.xlsx
+++ b/TPV_Source/test2.xlsx
@@ -34,7 +34,7 @@
     <t>Annet:</t>
   </si>
   <si>
-    <t>17.04.2018, Tue</t>
+    <t>18.04.2018, Wed</t>
   </si>
 </sst>
 </file>
@@ -604,51 +604,51 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="n">
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>